<commit_message>
Adicionando arquivos do curso de power query no excel
</commit_message>
<xml_diff>
--- a/Excel/my_first_workbook.xlsx
+++ b/Excel/my_first_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Documents\Projetos\Santander Ciência de Dados\desafios_de_codigo\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D8D018-B01F-43EC-BA84-02B56B4B2F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A5C39E-5549-4072-95EE-CFF6E6C301EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7B2FD790-3C15-411E-B526-84DE653427C9}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-416]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -207,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -215,75 +215,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color theme="0"/>
@@ -533,6 +465,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="403545056"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1670,13 +1603,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E15">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$E6="Stuck"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$E6="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$E6="Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>